<commit_message>
checkpoint g13; feito t13.1
</commit_message>
<xml_diff>
--- a/Data/t13.1.xlsx
+++ b/Data/t13.1.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -387,16 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>79.04766161593587</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>78.18785334283159</v>
       </c>
     </row>
     <row r="3">
@@ -407,16 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>79.67335137194378</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>79.04766161593587</v>
       </c>
     </row>
     <row r="4">
@@ -427,16 +503,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>80.16927727925945</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>79.67335137194378</v>
       </c>
     </row>
     <row r="5">
@@ -447,16 +523,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>80.596605163257</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>80.16927727925945</v>
       </c>
     </row>
     <row r="6">
@@ -467,16 +543,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>80.9366717682631</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>80.596605163257</v>
       </c>
     </row>
     <row r="7">
@@ -487,16 +563,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>81.2474962126619</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>80.9366717682631</v>
       </c>
     </row>
     <row r="8">
@@ -507,16 +583,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>49.27516798522028</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>81.2474962126619</v>
       </c>
     </row>
     <row r="9">
@@ -527,16 +603,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>49.80707803815459</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>45.6320636989658</v>
       </c>
     </row>
     <row r="10">
@@ -547,16 +623,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>50.76588115985216</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>45.89212195255193</v>
       </c>
     </row>
     <row r="11">
@@ -567,16 +643,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>46.40541129024624</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>43.86947730358591</v>
       </c>
     </row>
     <row r="12">
@@ -587,16 +663,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>50.73397663219978</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>44.66478580800823</v>
       </c>
     </row>
     <row r="13">
@@ -607,16 +683,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>50.66514405698735</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>39.49550794747753</v>
       </c>
     </row>
     <row r="14">
@@ -627,16 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>45.89212195255193</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>46.31985143155773</v>
       </c>
     </row>
     <row r="15">
@@ -647,16 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>43.86947730358591</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>47.44141713212169</v>
       </c>
     </row>
     <row r="16">
@@ -667,16 +743,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D16">
-        <v>44.66478580800823</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>3.507282840990042</v>
       </c>
     </row>
     <row r="17">
@@ -687,16 +763,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D17">
-        <v>39.49550794747753</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>3.383046032668345</v>
       </c>
     </row>
     <row r="18">
@@ -707,16 +783,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D18">
-        <v>46.31985143155773</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>5.937112324538696</v>
       </c>
     </row>
     <row r="19">
@@ -727,16 +803,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D19">
-        <v>47.44141713212169</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>6.101095351843931</v>
       </c>
     </row>
     <row r="20">
@@ -747,16 +823,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D20">
-        <v>3.383046032668345</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6.909903342768694</v>
       </c>
     </row>
     <row r="21">
@@ -767,16 +843,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D21">
-        <v>5.937112324538696</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.414125200642054</v>
       </c>
     </row>
     <row r="22">
@@ -787,16 +863,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D22">
-        <v>6.101095351843931</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.223726924865659</v>
       </c>
     </row>
     <row r="23">
@@ -807,16 +883,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D23">
-        <v>6.909903342768694</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>29.04850680287575</v>
       </c>
     </row>
     <row r="24">
@@ -827,16 +903,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D24">
-        <v>4.414125200642054</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>29.7724936307156</v>
       </c>
     </row>
     <row r="25">
@@ -847,16 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D25">
-        <v>3.223726924865659</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>29.86676174381917</v>
       </c>
     </row>
     <row r="26">
@@ -867,16 +943,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D26">
-        <v>29.7724936307156</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>29.40339611940729</v>
       </c>
     </row>
     <row r="27">
@@ -887,16 +963,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D27">
-        <v>29.86676174381917</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>34.19166721890355</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +983,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D28">
-        <v>29.40339611940729</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>30.20316174549255</v>
       </c>
     </row>
     <row r="29">
@@ -927,16 +1003,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D29">
-        <v>34.19166721890355</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>30.58235215567456</v>
       </c>
     </row>
     <row r="30">
@@ -947,16 +1023,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D30">
-        <v>30.20316174549255</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>49.13884131338699</v>
       </c>
     </row>
     <row r="31">
@@ -967,113 +1043,116 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D31">
-        <v>30.58235215567456</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>49.27516798522028</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D32">
-        <v>76.77104954426495</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>49.80707803815459</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D33">
-        <v>77.96395431834404</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>50.76588115985216</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D34">
-        <v>78.62626405237985</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>46.40541129024624</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>50.73397663219978</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D36">
-        <v>79.771414738735</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>50.66514405698735</v>
       </c>
     </row>
     <row r="37">
@@ -1084,16 +1163,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D37">
-        <v>80.25357662982952</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>75.84632801373115</v>
       </c>
     </row>
     <row r="38">
@@ -1104,7 +1183,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1112,8 +1191,8 @@
           <t>01/07/2014</t>
         </is>
       </c>
-      <c r="D38">
-        <v>44.51764281202058</v>
+      <c r="D38" t="n">
+        <v>76.77104954426495</v>
       </c>
     </row>
     <row r="39">
@@ -1124,7 +1203,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1132,8 +1211,8 @@
           <t>01/07/2016</t>
         </is>
       </c>
-      <c r="D39">
-        <v>43.76695217701641</v>
+      <c r="D39" t="n">
+        <v>77.96395431834404</v>
       </c>
     </row>
     <row r="40">
@@ -1144,7 +1223,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1152,8 +1231,8 @@
           <t>01/07/2018</t>
         </is>
       </c>
-      <c r="D40">
-        <v>44.13991493567231</v>
+      <c r="D40" t="n">
+        <v>78.62626405237985</v>
       </c>
     </row>
     <row r="41">
@@ -1164,13 +1243,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>01/07/2020</t>
         </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1181,7 +1263,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1189,8 +1271,8 @@
           <t>01/07/2022</t>
         </is>
       </c>
-      <c r="D42">
-        <v>43.96375834284331</v>
+      <c r="D42" t="n">
+        <v>79.771414738735</v>
       </c>
     </row>
     <row r="43">
@@ -1201,7 +1283,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1209,8 +1291,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D43">
-        <v>43.92015762871584</v>
+      <c r="D43" t="n">
+        <v>80.25357662982952</v>
       </c>
     </row>
     <row r="44">
@@ -1221,16 +1303,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D44">
-        <v>40.65517552567458</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>39.89519044662747</v>
       </c>
     </row>
     <row r="45">
@@ -1241,16 +1323,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D45">
-        <v>37.52498215560314</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>40.65517552567458</v>
       </c>
     </row>
     <row r="46">
@@ -1261,16 +1343,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D46">
-        <v>37.70185129626034</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>37.52498215560314</v>
       </c>
     </row>
     <row r="47">
@@ -1281,13 +1363,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>37.70185129626034</v>
       </c>
     </row>
     <row r="48">
@@ -1298,16 +1383,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D48">
-        <v>38.70041843898053</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1318,16 +1403,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D49">
-        <v>40.11136811445215</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>38.70041843898053</v>
       </c>
     </row>
     <row r="50">
@@ -1338,16 +1423,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D50">
-        <v>3.862467286345998</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>40.11136811445215</v>
       </c>
     </row>
     <row r="51">
@@ -1358,16 +1443,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D51">
-        <v>6.241970021413276</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>4.163166928386225</v>
       </c>
     </row>
     <row r="52">
@@ -1378,16 +1463,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D52">
-        <v>6.436298819335369</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>3.862467286345998</v>
       </c>
     </row>
     <row r="53">
@@ -1398,13 +1483,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>6.241970021413276</v>
       </c>
     </row>
     <row r="54">
@@ -1415,16 +1503,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D54">
-        <v>5.26333990386278</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>6.436298819335369</v>
       </c>
     </row>
     <row r="55">
@@ -1435,16 +1523,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>3.808789514263686</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1455,16 +1543,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D56">
-        <v>32.25340673224439</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>5.26333990386278</v>
       </c>
     </row>
     <row r="57">
@@ -1475,16 +1563,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D57">
-        <v>34.19700214132762</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>3.808789514263686</v>
       </c>
     </row>
     <row r="58">
@@ -1495,16 +1583,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D58">
-        <v>34.48811393678415</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>31.78797063871745</v>
       </c>
     </row>
     <row r="59">
@@ -1515,13 +1603,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>32.25340673224439</v>
       </c>
     </row>
     <row r="60">
@@ -1532,16 +1623,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D60">
-        <v>35.80765639589169</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>34.19700214132762</v>
       </c>
     </row>
     <row r="61">
@@ -1552,210 +1643,216 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D61">
-        <v>36.33341900111368</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>34.48811393678415</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D62">
-        <v>76.55894401456531</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D63">
-        <v>78.83928571428571</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>35.80765639589169</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D64">
-        <v>77.77290661990355</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>36.33341900111368</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>44.0583573750137</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D66">
-        <v>79.11016949152543</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>44.51764281202058</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D67">
-        <v>79.96661101836395</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>43.76695217701641</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D68">
-        <v>46.15384615384615</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>44.13991493567231</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D69">
-        <v>45.80357142857142</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D70">
-        <v>45.46251644015783</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>43.96375834284331</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>43.92015762871584</v>
       </c>
     </row>
     <row r="72">
@@ -1766,16 +1863,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D72">
-        <v>45.76271186440678</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>75.5803156917363</v>
       </c>
     </row>
     <row r="73">
@@ -1786,16 +1883,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D73">
-        <v>46.78631051752922</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>76.55894401456531</v>
       </c>
     </row>
     <row r="74">
@@ -1806,16 +1903,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D74">
-        <v>41.92080109239873</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>78.83928571428571</v>
       </c>
     </row>
     <row r="75">
@@ -1826,16 +1923,16 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D75">
-        <v>39.15178571428572</v>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>77.77290661990355</v>
       </c>
     </row>
     <row r="76">
@@ -1846,16 +1943,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D76">
-        <v>37.48355984217449</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1866,13 +1963,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>79.11016949152543</v>
       </c>
     </row>
     <row r="78">
@@ -1883,16 +1983,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D78">
-        <v>40.21186440677966</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>79.96661101836395</v>
       </c>
     </row>
     <row r="79">
@@ -1903,16 +2003,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D79">
-        <v>42.86310517529216</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>40.99350046425256</v>
       </c>
     </row>
     <row r="80">
@@ -1923,7 +2023,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1931,8 +2031,8 @@
           <t>01/07/2014</t>
         </is>
       </c>
-      <c r="D80">
-        <v>4.233045061447428</v>
+      <c r="D80" t="n">
+        <v>41.92080109239873</v>
       </c>
     </row>
     <row r="81">
@@ -1943,7 +2043,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1951,8 +2051,8 @@
           <t>01/07/2016</t>
         </is>
       </c>
-      <c r="D81">
-        <v>6.607142857142858</v>
+      <c r="D81" t="n">
+        <v>39.15178571428572</v>
       </c>
     </row>
     <row r="82">
@@ -1963,7 +2063,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1971,8 +2071,8 @@
           <t>01/07/2018</t>
         </is>
       </c>
-      <c r="D82">
-        <v>8.022797018851382</v>
+      <c r="D82" t="n">
+        <v>37.48355984217449</v>
       </c>
     </row>
     <row r="83">
@@ -1983,13 +2083,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>01/07/2020</t>
         </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2000,7 +2103,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2008,8 +2111,8 @@
           <t>01/07/2022</t>
         </is>
       </c>
-      <c r="D84">
-        <v>5.550847457627119</v>
+      <c r="D84" t="n">
+        <v>40.21186440677966</v>
       </c>
     </row>
     <row r="85">
@@ -2020,7 +2123,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade ocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2028,8 +2131,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D85">
-        <v>3.923205342237062</v>
+      <c r="D85" t="n">
+        <v>42.86310517529216</v>
       </c>
     </row>
     <row r="86">
@@ -2040,16 +2143,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>01/07/2014</t>
-        </is>
-      </c>
-      <c r="D86">
-        <v>30.40509786071916</v>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>4.874651810584958</v>
       </c>
     </row>
     <row r="87">
@@ -2060,16 +2163,16 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>01/07/2016</t>
-        </is>
-      </c>
-      <c r="D87">
-        <v>33.03571428571428</v>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>4.233045061447428</v>
       </c>
     </row>
     <row r="88">
@@ -2080,16 +2183,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>01/07/2018</t>
-        </is>
-      </c>
-      <c r="D88">
-        <v>32.26654975887768</v>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>6.607142857142858</v>
       </c>
     </row>
     <row r="89">
@@ -2100,13 +2203,16 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>8.022797018851382</v>
       </c>
     </row>
     <row r="90">
@@ -2117,16 +2223,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D90">
-        <v>33.34745762711864</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2137,19 +2243,319 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>5.550847457627119</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, desocupadas na semana de referência</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D91">
+      <c r="D92" t="n">
+        <v>3.923205342237062</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>29.71216341689879</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>30.40509786071916</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>33.03571428571428</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>32.26654975887768</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>33.34745762711864</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, fora da força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
         <v>33.13856427378965</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>01/07/2012</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>45.86815227483751</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>01/07/2014</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>46.15384615384615</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>01/07/2016</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>45.80357142857142</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>01/07/2018</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>45.46251644015783</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>45.76271186440678</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>46.78631051752922</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>